<commit_message>
added show hide feature
</commit_message>
<xml_diff>
--- a/calculated_tables_t.xlsx
+++ b/calculated_tables_t.xlsx
@@ -487,22 +487,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-31.46</v>
+        <v>12.15</v>
       </c>
       <c r="D2" t="n">
-        <v>1.89999999999993</v>
+        <v>1.899999999999995</v>
       </c>
       <c r="E2" t="n">
-        <v>-9.800000000000072</v>
+        <v>-9.800000000000001</v>
       </c>
       <c r="F2" t="n">
-        <v>20.69999999999993</v>
+        <v>20.7</v>
       </c>
       <c r="G2" t="n">
-        <v>16.09999999999993</v>
+        <v>16.1</v>
       </c>
       <c r="H2" t="n">
-        <v>-8.90000000000007</v>
+        <v>-8.9</v>
       </c>
     </row>
     <row r="3">
@@ -518,19 +518,19 @@
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
-        <v>-6.700000000000069</v>
+        <v>-6.700000000000005</v>
       </c>
       <c r="E3" t="n">
-        <v>2.09999999999993</v>
+        <v>2.1</v>
       </c>
       <c r="F3" t="n">
-        <v>25.69999999999993</v>
+        <v>25.7</v>
       </c>
       <c r="G3" t="n">
-        <v>16.09999999999993</v>
+        <v>16.1</v>
       </c>
       <c r="H3" t="n">
-        <v>15.39999999999993</v>
+        <v>15.4</v>
       </c>
     </row>
     <row r="4">
@@ -546,19 +546,19 @@
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
-        <v>1.89999999999993</v>
+        <v>1.899999999999995</v>
       </c>
       <c r="E4" t="n">
-        <v>-9.800000000000072</v>
+        <v>-9.800000000000001</v>
       </c>
       <c r="F4" t="n">
-        <v>20.69999999999993</v>
+        <v>20.7</v>
       </c>
       <c r="G4" t="n">
-        <v>16.09999999999993</v>
+        <v>16.1</v>
       </c>
       <c r="H4" t="n">
-        <v>-8.90000000000007</v>
+        <v>-8.9</v>
       </c>
     </row>
     <row r="5">
@@ -574,19 +574,19 @@
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
-        <v>-6.700000000000069</v>
+        <v>-6.700000000000005</v>
       </c>
       <c r="E5" t="n">
-        <v>2.09999999999993</v>
+        <v>2.1</v>
       </c>
       <c r="F5" t="n">
-        <v>25.69999999999993</v>
+        <v>25.7</v>
       </c>
       <c r="G5" t="n">
-        <v>16.09999999999993</v>
+        <v>16.1</v>
       </c>
       <c r="H5" t="n">
-        <v>15.39999999999993</v>
+        <v>15.4</v>
       </c>
     </row>
     <row r="6">
@@ -602,19 +602,19 @@
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
-        <v>1.89999999999993</v>
+        <v>1.899999999999995</v>
       </c>
       <c r="E6" t="n">
-        <v>-9.800000000000072</v>
+        <v>-9.800000000000001</v>
       </c>
       <c r="F6" t="n">
-        <v>20.69999999999993</v>
+        <v>20.7</v>
       </c>
       <c r="G6" t="n">
-        <v>16.09999999999993</v>
+        <v>16.1</v>
       </c>
       <c r="H6" t="n">
-        <v>-8.90000000000007</v>
+        <v>-8.9</v>
       </c>
     </row>
     <row r="7">
@@ -630,19 +630,19 @@
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
-        <v>-6.700000000000069</v>
+        <v>-6.700000000000005</v>
       </c>
       <c r="E7" t="n">
-        <v>2.09999999999993</v>
+        <v>2.1</v>
       </c>
       <c r="F7" t="n">
-        <v>25.69999999999993</v>
+        <v>25.7</v>
       </c>
       <c r="G7" t="n">
-        <v>16.09999999999993</v>
+        <v>16.1</v>
       </c>
       <c r="H7" t="n">
-        <v>15.39999999999993</v>
+        <v>15.4</v>
       </c>
     </row>
     <row r="8">
@@ -658,19 +658,19 @@
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
-        <v>-6.700000000000069</v>
+        <v>-6.700000000000005</v>
       </c>
       <c r="E8" t="n">
-        <v>2.09999999999993</v>
+        <v>2.1</v>
       </c>
       <c r="F8" t="n">
-        <v>25.69999999999993</v>
+        <v>25.7</v>
       </c>
       <c r="G8" t="n">
-        <v>16.09999999999993</v>
+        <v>16.1</v>
       </c>
       <c r="H8" t="n">
-        <v>15.39999999999993</v>
+        <v>15.4</v>
       </c>
     </row>
     <row r="9">
@@ -686,19 +686,19 @@
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="n">
-        <v>1.89999999999993</v>
+        <v>1.899999999999995</v>
       </c>
       <c r="E9" t="n">
-        <v>-9.800000000000072</v>
+        <v>-9.800000000000001</v>
       </c>
       <c r="F9" t="n">
-        <v>20.69999999999993</v>
+        <v>20.7</v>
       </c>
       <c r="G9" t="n">
-        <v>16.09999999999993</v>
+        <v>16.1</v>
       </c>
       <c r="H9" t="n">
-        <v>-8.90000000000007</v>
+        <v>-8.9</v>
       </c>
     </row>
     <row r="10">
@@ -714,19 +714,19 @@
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
-        <v>-6.700000000000069</v>
+        <v>-6.700000000000005</v>
       </c>
       <c r="E10" t="n">
-        <v>2.09999999999993</v>
+        <v>2.1</v>
       </c>
       <c r="F10" t="n">
-        <v>25.69999999999993</v>
+        <v>25.7</v>
       </c>
       <c r="G10" t="n">
-        <v>16.09999999999993</v>
+        <v>16.1</v>
       </c>
       <c r="H10" t="n">
-        <v>15.39999999999993</v>
+        <v>15.4</v>
       </c>
     </row>
     <row r="11">
@@ -742,19 +742,19 @@
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="n">
-        <v>1.89999999999993</v>
+        <v>1.899999999999995</v>
       </c>
       <c r="E11" t="n">
-        <v>-9.800000000000072</v>
+        <v>-9.800000000000001</v>
       </c>
       <c r="F11" t="n">
-        <v>20.69999999999993</v>
+        <v>20.7</v>
       </c>
       <c r="G11" t="n">
-        <v>16.09999999999993</v>
+        <v>16.1</v>
       </c>
       <c r="H11" t="n">
-        <v>-8.90000000000007</v>
+        <v>-8.9</v>
       </c>
     </row>
     <row r="12">
@@ -770,19 +770,19 @@
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="n">
-        <v>-6.700000000000069</v>
+        <v>-6.700000000000005</v>
       </c>
       <c r="E12" t="n">
-        <v>2.09999999999993</v>
+        <v>2.1</v>
       </c>
       <c r="F12" t="n">
-        <v>25.69999999999993</v>
+        <v>25.7</v>
       </c>
       <c r="G12" t="n">
-        <v>16.09999999999993</v>
+        <v>16.1</v>
       </c>
       <c r="H12" t="n">
-        <v>15.39999999999993</v>
+        <v>15.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>